<commit_message>
add multiplication of distributions according to the product rule
</commit_message>
<xml_diff>
--- a/tests/test_data/pandas-test-data.xlsx
+++ b/tests/test_data/pandas-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahndi.minah/Desktop/gitcode/dev/probability/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1585241D-8C66-2944-9354-E89DCD660022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905AC91B-9F87-9F4B-9C00-0B63B901883A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="-25880" windowWidth="25260" windowHeight="20760" activeTab="9" xr2:uid="{C4B7374F-96C9-B341-8E2A-ECD5F364454A}"/>
+    <workbookView xWindow="34440" yWindow="-33840" windowWidth="27200" windowHeight="24040" activeTab="11" xr2:uid="{C4B7374F-96C9-B341-8E2A-ECD5F364454A}"/>
   </bookViews>
   <sheets>
     <sheet name="P(A,B,C,D)" sheetId="3" r:id="rId1"/>
@@ -23,8 +23,11 @@
     <sheet name="p(A,B,C|D)" sheetId="10" r:id="rId8"/>
     <sheet name="p(A,B|C,D)" sheetId="11" r:id="rId9"/>
     <sheet name="P(A|B,C,D)" sheetId="12" r:id="rId10"/>
+    <sheet name="p(A,B|C,D=1)" sheetId="13" r:id="rId11"/>
+    <sheet name="p(A,B|C=2,D)" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'p(A,B|C=2,D)'!$A$1:$F$28</definedName>
     <definedName name="pABCD">'P(A,B,C,D)'!$E:$E</definedName>
     <definedName name="pABCD_A">'P(A,B,C,D)'!$A:$A</definedName>
     <definedName name="pABCD_B">'P(A,B,C,D)'!$B:$B</definedName>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="6">
   <si>
     <t>p</t>
   </si>
@@ -1485,7 +1488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B7ACF4-B9D5-8647-97DB-18595615245A}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
@@ -3295,6 +3298,1271 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72C3FDF-7439-414E-A654-92B338B357A1}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:E28" si="0">SUMIFS(pABCD,pABCD_A,A2,pABCD_B,B2,pABCD_C,C2,pABCD_D,D2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>E2/SUM(E$2:E$10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="1">E3/SUM(E$2:E$10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F11">
+        <f>E11/SUM(E$11:E$19)</f>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F19" si="2">E12/SUM(E$11:E$19)</f>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>E20/SUM(E$20:E$28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F28" si="3">E21/SUM(E$20:E$28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926797A6-DB0A-B64F-9644-731023A768AB}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A2,pABCD_B,B2,pABCD_C,C2,pABCD_D,D2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F2">
+        <f>E2/SUM(E$2:E$10)</f>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A3,pABCD_B,B3,pABCD_C,C3,pABCD_D,D3)</f>
+        <v>0.02</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="0">E3/SUM(E$2:E$10)</f>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A4,pABCD_B,B4,pABCD_C,C4,pABCD_D,D4)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A5,pABCD_B,B5,pABCD_C,C5,pABCD_D,D5)</f>
+        <v>0.02</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A6,pABCD_B,B6,pABCD_C,C6,pABCD_D,D6)</f>
+        <v>0.02</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A7,pABCD_B,B7,pABCD_C,C7,pABCD_D,D7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A8,pABCD_B,B8,pABCD_C,C8,pABCD_D,D8)</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A9,pABCD_B,B9,pABCD_C,C9,pABCD_D,D9)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A10,pABCD_B,B10,pABCD_C,C10,pABCD_D,D10)</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A11,pABCD_B,B11,pABCD_C,C11,pABCD_D,D11)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F11">
+        <f>E11/SUM(E$11:E$19)</f>
+        <v>8.3333333333333343E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A12,pABCD_B,B12,pABCD_C,C12,pABCD_D,D12)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F19" si="1">E12/SUM(E$11:E$19)</f>
+        <v>8.3333333333333343E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A13,pABCD_B,B13,pABCD_C,C13,pABCD_D,D13)</f>
+        <v>0.02</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A14,pABCD_B,B14,pABCD_C,C14,pABCD_D,D14)</f>
+        <v>0.02</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A15,pABCD_B,B15,pABCD_C,C15,pABCD_D,D15)</f>
+        <v>0.03</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A16,pABCD_B,B16,pABCD_C,C16,pABCD_D,D16)</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A17,pABCD_B,B17,pABCD_C,C17,pABCD_D,D17)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333343E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A18,pABCD_B,B18,pABCD_C,C18,pABCD_D,D18)</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A19,pABCD_B,B19,pABCD_C,C19,pABCD_D,D19)</f>
+        <v>0.02</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666669</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A20,pABCD_B,B20,pABCD_C,C20,pABCD_D,D20)</f>
+        <v>0.03</v>
+      </c>
+      <c r="F20">
+        <f>E20/SUM(E$20:E$28)</f>
+        <v>0.21428571428571425</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A21,pABCD_B,B21,pABCD_C,C21,pABCD_D,D21)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F28" si="2">E21/SUM(E$20:E$28)</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A22,pABCD_B,B22,pABCD_C,C22,pABCD_D,D22)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A23,pABCD_B,B23,pABCD_C,C23,pABCD_D,D23)</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A24,pABCD_B,B24,pABCD_C,C24,pABCD_D,D24)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A25,pABCD_B,B25,pABCD_C,C25,pABCD_D,D25)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A26,pABCD_B,B26,pABCD_C,C26,pABCD_D,D26)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3</v>
+      </c>
+      <c r="E27" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A27,pABCD_B,B27,pABCD_C,C27,pABCD_D,D27)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3</v>
+      </c>
+      <c r="E28" s="1">
+        <f>SUMIFS(pABCD,pABCD_A,A28,pABCD_B,B28,pABCD_C,C28,pABCD_D,D28)</f>
+        <v>0.05</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F28" xr:uid="{187070E8-FB97-F545-9C9A-803A3205811E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
+      <sortCondition ref="C1:C28"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5258,7 +6526,7 @@
         <v>0.01</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F29" si="1">E3/SUM(E$2:E$28)</f>
+        <f t="shared" ref="F3:F28" si="1">E3/SUM(E$2:E$28)</f>
         <v>0.04</v>
       </c>
     </row>
@@ -5852,7 +7120,7 @@
         <v>0.01</v>
       </c>
       <c r="F30">
-        <f t="shared" ref="F30:F82" si="2">E30/SUM(E$29:E$55)</f>
+        <f t="shared" ref="F30:F55" si="2">E30/SUM(E$29:E$55)</f>
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
@@ -7274,7 +8542,7 @@
         <v>0.02</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F75" si="2">E12/SUM(E$11:E$19)</f>
+        <f t="shared" ref="F12:F19" si="2">E12/SUM(E$11:E$19)</f>
         <v>0.2857142857142857</v>
       </c>
     </row>
@@ -7472,7 +8740,7 @@
         <v>0.03</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F82" si="3">E21/SUM(E$20:E$28)</f>
+        <f t="shared" ref="F21:F28" si="3">E21/SUM(E$20:E$28)</f>
         <v>0.23076923076923081</v>
       </c>
     </row>
@@ -7670,7 +8938,7 @@
         <v>0.02</v>
       </c>
       <c r="F30">
-        <f t="shared" ref="F30:F82" si="4">E30/SUM(E$29:E$37)</f>
+        <f t="shared" ref="F30:F37" si="4">E30/SUM(E$29:E$37)</f>
         <v>0.22222222222222224</v>
       </c>
     </row>
@@ -7868,7 +9136,7 @@
         <v>0.01</v>
       </c>
       <c r="F39">
-        <f t="shared" ref="F39:F82" si="5">E39/SUM(E$38:E$46)</f>
+        <f t="shared" ref="F39:F46" si="5">E39/SUM(E$38:E$46)</f>
         <v>8.3333333333333343E-2</v>
       </c>
     </row>
@@ -8066,7 +9334,7 @@
         <v>0.01</v>
       </c>
       <c r="F48">
-        <f t="shared" ref="F48:F82" si="6">E48/SUM(E$47:E$55)</f>
+        <f t="shared" ref="F48:F55" si="6">E48/SUM(E$47:E$55)</f>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -8264,7 +9532,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <f t="shared" ref="F57:F82" si="7">E57/SUM(E$56:E$64)</f>
+        <f t="shared" ref="F57:F64" si="7">E57/SUM(E$56:E$64)</f>
         <v>0</v>
       </c>
     </row>
@@ -8462,7 +9730,7 @@
         <v>0.02</v>
       </c>
       <c r="F66">
-        <f t="shared" ref="F66:F82" si="9">E66/SUM(E$65:E$73)</f>
+        <f t="shared" ref="F66:F73" si="9">E66/SUM(E$65:E$73)</f>
         <v>0.13333333333333333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
write tests for remaining DiscreteDistribution and ConditionalTable methods
</commit_message>
<xml_diff>
--- a/tests/test_data/pandas-test-data.xlsx
+++ b/tests/test_data/pandas-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahndi.minah/Desktop/gitcode/dev/probability/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905AC91B-9F87-9F4B-9C00-0B63B901883A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA07838-4FC8-0344-8F94-21BB20ACBB07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34440" yWindow="-33840" windowWidth="27200" windowHeight="24040" activeTab="11" xr2:uid="{C4B7374F-96C9-B341-8E2A-ECD5F364454A}"/>
+    <workbookView xWindow="34440" yWindow="-33840" windowWidth="27200" windowHeight="24040" activeTab="6" xr2:uid="{C4B7374F-96C9-B341-8E2A-ECD5F364454A}"/>
   </bookViews>
   <sheets>
     <sheet name="P(A,B,C,D)" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="9">
   <si>
     <t>p</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>_p</t>
+  </si>
+  <si>
+    <t>_D</t>
+  </si>
+  <si>
+    <t>_C</t>
+  </si>
+  <si>
+    <t>_B</t>
   </si>
 </sst>
 </file>
@@ -3308,7 +3317,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F28"/>
+      <selection pane="bottomLeft" activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3324,7 +3333,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -3936,9 +3945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926797A6-DB0A-B64F-9644-731023A768AB}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3951,7 +3960,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -3977,7 +3986,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A2,pABCD_B,B2,pABCD_C,C2,pABCD_D,D2)</f>
+        <f t="shared" ref="E2:E28" si="0">SUMIFS(pABCD,pABCD_A,A2,pABCD_B,B2,pABCD_C,C2,pABCD_D,D2)</f>
         <v>0.01</v>
       </c>
       <c r="F2">
@@ -3999,11 +4008,11 @@
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A3,pABCD_B,B3,pABCD_C,C3,pABCD_D,D3)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F10" si="0">E3/SUM(E$2:E$10)</f>
+        <f t="shared" ref="F3:F10" si="1">E3/SUM(E$2:E$10)</f>
         <v>0.22222222222222224</v>
       </c>
     </row>
@@ -4021,11 +4030,11 @@
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A4,pABCD_B,B4,pABCD_C,C4,pABCD_D,D4)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11111111111111112</v>
       </c>
     </row>
@@ -4043,11 +4052,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A5,pABCD_B,B5,pABCD_C,C5,pABCD_D,D5)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.22222222222222224</v>
       </c>
     </row>
@@ -4065,11 +4074,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A6,pABCD_B,B6,pABCD_C,C6,pABCD_D,D6)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.22222222222222224</v>
       </c>
     </row>
@@ -4087,11 +4096,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A7,pABCD_B,B7,pABCD_C,C7,pABCD_D,D7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4109,11 +4118,11 @@
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A8,pABCD_B,B8,pABCD_C,C8,pABCD_D,D8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4131,11 +4140,11 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A9,pABCD_B,B9,pABCD_C,C9,pABCD_D,D9)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11111111111111112</v>
       </c>
     </row>
@@ -4153,11 +4162,11 @@
         <v>1</v>
       </c>
       <c r="E10" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A10,pABCD_B,B10,pABCD_C,C10,pABCD_D,D10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4175,7 +4184,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A11,pABCD_B,B11,pABCD_C,C11,pABCD_D,D11)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F11">
@@ -4197,11 +4206,11 @@
         <v>2</v>
       </c>
       <c r="E12" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A12,pABCD_B,B12,pABCD_C,C12,pABCD_D,D12)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F19" si="1">E12/SUM(E$11:E$19)</f>
+        <f t="shared" ref="F12:F19" si="2">E12/SUM(E$11:E$19)</f>
         <v>8.3333333333333343E-2</v>
       </c>
     </row>
@@ -4219,11 +4228,11 @@
         <v>2</v>
       </c>
       <c r="E13" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A13,pABCD_B,B13,pABCD_C,C13,pABCD_D,D13)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16666666666666669</v>
       </c>
     </row>
@@ -4241,11 +4250,11 @@
         <v>2</v>
       </c>
       <c r="E14" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A14,pABCD_B,B14,pABCD_C,C14,pABCD_D,D14)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16666666666666669</v>
       </c>
     </row>
@@ -4263,11 +4272,11 @@
         <v>2</v>
       </c>
       <c r="E15" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A15,pABCD_B,B15,pABCD_C,C15,pABCD_D,D15)</f>
+        <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
     </row>
@@ -4285,11 +4294,11 @@
         <v>2</v>
       </c>
       <c r="E16" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A16,pABCD_B,B16,pABCD_C,C16,pABCD_D,D16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4307,11 +4316,11 @@
         <v>2</v>
       </c>
       <c r="E17" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A17,pABCD_B,B17,pABCD_C,C17,pABCD_D,D17)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3333333333333343E-2</v>
       </c>
     </row>
@@ -4329,11 +4338,11 @@
         <v>2</v>
       </c>
       <c r="E18" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A18,pABCD_B,B18,pABCD_C,C18,pABCD_D,D18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4351,11 +4360,11 @@
         <v>2</v>
       </c>
       <c r="E19" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A19,pABCD_B,B19,pABCD_C,C19,pABCD_D,D19)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16666666666666669</v>
       </c>
     </row>
@@ -4373,7 +4382,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A20,pABCD_B,B20,pABCD_C,C20,pABCD_D,D20)</f>
+        <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
       <c r="F20">
@@ -4395,11 +4404,11 @@
         <v>3</v>
       </c>
       <c r="E21" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A21,pABCD_B,B21,pABCD_C,C21,pABCD_D,D21)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F28" si="2">E21/SUM(E$20:E$28)</f>
+        <f t="shared" ref="F21:F28" si="3">E21/SUM(E$20:E$28)</f>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -4417,11 +4426,11 @@
         <v>3</v>
       </c>
       <c r="E22" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A22,pABCD_B,B22,pABCD_C,C22,pABCD_D,D22)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -4439,11 +4448,11 @@
         <v>3</v>
       </c>
       <c r="E23" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A23,pABCD_B,B23,pABCD_C,C23,pABCD_D,D23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4461,11 +4470,11 @@
         <v>3</v>
       </c>
       <c r="E24" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A24,pABCD_B,B24,pABCD_C,C24,pABCD_D,D24)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -4483,11 +4492,11 @@
         <v>3</v>
       </c>
       <c r="E25" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A25,pABCD_B,B25,pABCD_C,C25,pABCD_D,D25)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -4505,11 +4514,11 @@
         <v>3</v>
       </c>
       <c r="E26" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A26,pABCD_B,B26,pABCD_C,C26,pABCD_D,D26)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -4527,11 +4536,11 @@
         <v>3</v>
       </c>
       <c r="E27" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A27,pABCD_B,B27,pABCD_C,C27,pABCD_D,D27)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -4549,11 +4558,11 @@
         <v>3</v>
       </c>
       <c r="E28" s="1">
-        <f>SUMIFS(pABCD,pABCD_A,A28,pABCD_B,B28,pABCD_C,C28,pABCD_D,D28)</f>
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.35714285714285715</v>
       </c>
     </row>
@@ -5197,7 +5206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F1"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5213,7 +5222,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -6083,7 +6092,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6096,10 +6105,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -6315,9 +6324,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A916DC3-10D3-E94A-A13F-9011078C3B44}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6327,13 +6336,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>

</xml_diff>